<commit_message>
Added coefficient interpolation. this fixed the aoa locking problem. simulation now seems perfectly smooth and is marginally stable, but not perfectly stable. hard to tell why but probably due to improper implementation of drag coefficient table
</commit_message>
<xml_diff>
--- a/Aero design/Flight sim/hover stage sim - RK4 method/lookupTableCl.xlsx
+++ b/Aero design/Flight sim/hover stage sim - RK4 method/lookupTableCl.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joseph\Documents\Crash-Sat\Crash-Sat\Aero design\Flight sim\hover stage sim - RK4 method\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D853CBF8-42AE-4A6C-8C05-CD89D9F2671C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EECB3EE4-B80D-4FF8-A203-BFA9E5473204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -351,7 +351,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:K14"/>
+      <selection activeCell="A2" sqref="A2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -384,28 +384,28 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>-0.15</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>-0.39600000000000002</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>-0.6</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>-0.6</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>-0.6</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>-0.6</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>-0.6</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>-0.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -670,28 +670,28 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="B13">
-        <v>0.33</v>
+        <v>0</v>
       </c>
       <c r="C13">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D13">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F13">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G13">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H13">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>